<commit_message>
update style of Data
</commit_message>
<xml_diff>
--- a/기록/Data.xlsx
+++ b/기록/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\매일매일\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\CS_study\기록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633DEE36-9958-4AA9-955F-D107C0AA58B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73D7997-F3BE-4DD4-95C4-EBE493085E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="188">
   <si>
     <t>날짜</t>
   </si>
@@ -582,6 +582,14 @@
   </si>
   <si>
     <t>그래픽스</t>
+  </si>
+  <si>
+    <t>캡스톤 디자인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -696,12 +704,49 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -759,27 +804,6 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="11" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
@@ -805,6 +829,27 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="20% - 강조색1" xfId="1" builtinId="30"/>
@@ -821,7 +866,117 @@
     <cellStyle name="60% - 강조색2" xfId="6" builtinId="36"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="91">
+  <dxfs count="211">
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAFBD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -837,23 +992,120 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.89996032593768116"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAFBD5"/>
-        </patternFill>
-      </fill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFA4193D"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDFB9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF6A7BA2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDFDE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFDDA94B"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1E4174"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -908,69 +1160,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14990691854609822"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1008,12 +1197,189 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
+        <color rgb="FFA4193D"/>
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFDFB9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF6A7BA2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFDFDE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAFBD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF002060"/>
         </patternFill>
       </fill>
@@ -1021,11 +1387,358 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFF193E4"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAFBD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="8" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAFBD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.89996032593768116"/>
@@ -1035,6 +1748,182 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="8" tint="0.39994506668294322"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFAFBD5"/>
         </patternFill>
       </fill>
@@ -1042,6 +1931,133 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-0.14990691854609822"/>
         </patternFill>
       </fill>
@@ -1098,6 +2114,39 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFAFBD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1105,6 +2154,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1138,6 +2194,9 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
@@ -1152,6 +2211,128 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAFBD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
@@ -1161,6 +2342,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -1210,11 +2398,186 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAFBD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14990691854609822"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAFBD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="3" tint="0.89996032593768116"/>
@@ -1224,252 +2587,26 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFAFBD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14990691854609822"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.89996032593768116"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAFBD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14990691854609822"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAFBD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14990691854609822"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14990691854609822"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1477,6 +2614,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFDDA94B"/>
+      <color rgb="FF1E4174"/>
+      <color rgb="FFFFDFB9"/>
+      <color rgb="FFA4193D"/>
+      <color rgb="FF6A7BA2"/>
+      <color rgb="FFFFDFDE"/>
+      <color rgb="FFF193E4"/>
       <color rgb="FFFAFBD5"/>
     </mruColors>
   </colors>
@@ -1878,11 +3022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J160"/>
+  <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1892,32 +3035,32 @@
     <col min="3" max="3" width="5.875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59.25" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.875" style="19" customWidth="1"/>
-    <col min="9" max="9" width="9.125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="22.25" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I1"/>
@@ -1976,7 +3119,7 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -2057,7 +3200,7 @@
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="11" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -3487,7 +4630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>45292</v>
       </c>
@@ -3507,7 +4650,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>45292</v>
       </c>
@@ -3527,7 +4670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>45292</v>
       </c>
@@ -3547,7 +4690,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>45292</v>
       </c>
@@ -3567,7 +4710,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>45292</v>
       </c>
@@ -3587,7 +4730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>45292</v>
       </c>
@@ -3604,7 +4747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>45293</v>
       </c>
@@ -3624,7 +4767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>45293</v>
       </c>
@@ -3644,7 +4787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>45293</v>
       </c>
@@ -3664,7 +4807,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>45293</v>
       </c>
@@ -3684,7 +4827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>45293</v>
       </c>
@@ -3701,7 +4844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>45293</v>
       </c>
@@ -3718,7 +4861,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>45293</v>
       </c>
@@ -3735,7 +4878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>45294</v>
       </c>
@@ -3755,7 +4898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>45294</v>
       </c>
@@ -3772,7 +4915,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>45294</v>
       </c>
@@ -3789,7 +4932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>45294</v>
       </c>
@@ -3806,7 +4949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>45294</v>
       </c>
@@ -3823,7 +4966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>45294</v>
       </c>
@@ -3840,7 +4983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>45294</v>
       </c>
@@ -3857,7 +5000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>45294</v>
       </c>
@@ -3874,7 +5017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>45295</v>
       </c>
@@ -3894,7 +5037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>45295</v>
       </c>
@@ -3911,7 +5054,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>45295</v>
       </c>
@@ -3928,7 +5071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>45295</v>
       </c>
@@ -3945,7 +5088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>45295</v>
       </c>
@@ -3962,7 +5105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>45295</v>
       </c>
@@ -3979,7 +5122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>45295</v>
       </c>
@@ -3996,7 +5139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>45295</v>
       </c>
@@ -4013,7 +5156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>45295</v>
       </c>
@@ -4030,7 +5173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>45295</v>
       </c>
@@ -4047,7 +5190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>45296</v>
       </c>
@@ -4067,7 +5210,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>45296</v>
       </c>
@@ -4087,7 +5230,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>45296</v>
       </c>
@@ -4107,7 +5250,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>45296</v>
       </c>
@@ -4127,7 +5270,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>45296</v>
       </c>
@@ -4147,7 +5290,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>45296</v>
       </c>
@@ -4167,7 +5310,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>45296</v>
       </c>
@@ -4187,7 +5330,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>45323</v>
       </c>
@@ -4204,7 +5347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>45324</v>
       </c>
@@ -4221,7 +5364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>45324</v>
       </c>
@@ -4238,7 +5381,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>45325</v>
       </c>
@@ -4258,7 +5401,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>45325</v>
       </c>
@@ -4275,7 +5418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>45326</v>
       </c>
@@ -4295,7 +5438,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>45326</v>
       </c>
@@ -4312,7 +5455,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>45352</v>
       </c>
@@ -4332,7 +5475,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>45352</v>
       </c>
@@ -4352,7 +5495,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>45352</v>
       </c>
@@ -4372,7 +5515,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>45352</v>
       </c>
@@ -4389,7 +5532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>45353</v>
       </c>
@@ -4406,7 +5549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>45353</v>
       </c>
@@ -4426,7 +5569,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>45354</v>
       </c>
@@ -4446,7 +5589,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>45354</v>
       </c>
@@ -4463,7 +5606,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>45355</v>
       </c>
@@ -4483,7 +5626,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>45355</v>
       </c>
@@ -4500,7 +5643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>45326</v>
       </c>
@@ -4517,7 +5660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>45326</v>
       </c>
@@ -4534,7 +5677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>45352</v>
       </c>
@@ -4551,7 +5694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>45352</v>
       </c>
@@ -4568,7 +5711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>45352</v>
       </c>
@@ -4585,7 +5728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>45353</v>
       </c>
@@ -4602,7 +5745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>45353</v>
       </c>
@@ -4619,7 +5762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>45353</v>
       </c>
@@ -4636,7 +5779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>45353</v>
       </c>
@@ -4653,7 +5796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>45353</v>
       </c>
@@ -4670,7 +5813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>45353</v>
       </c>
@@ -4687,7 +5830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>45353</v>
       </c>
@@ -4704,7 +5847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>45353</v>
       </c>
@@ -4721,7 +5864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>45353</v>
       </c>
@@ -4738,7 +5881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>45354</v>
       </c>
@@ -4755,7 +5898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>45354</v>
       </c>
@@ -4772,7 +5915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>45354</v>
       </c>
@@ -4789,7 +5932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>45354</v>
       </c>
@@ -4806,7 +5949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>45355</v>
       </c>
@@ -4823,7 +5966,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>45355</v>
       </c>
@@ -4840,7 +5983,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>45355</v>
       </c>
@@ -4857,7 +6000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>45355</v>
       </c>
@@ -4874,7 +6017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>45355</v>
       </c>
@@ -4891,7 +6034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>45355</v>
       </c>
@@ -4908,86 +6051,84 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" spans="1:5" ht="17.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="A1:G160" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="김다은"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G160" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="52" priority="16">
+    <cfRule type="expression" dxfId="45" priority="18">
       <formula>(RIGHT(INDEX($A:$A, ROW()), 1)="1")*1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="51" priority="6" operator="containsText" text="김신영">
+    <cfRule type="containsText" dxfId="44" priority="8" operator="containsText" text="김신영">
       <formula>NOT(ISERROR(SEARCH("김신영",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="7" operator="containsText" text="박지훈">
+    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="박지훈">
       <formula>NOT(ISERROR(SEARCH("박지훈",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="8" operator="containsText" text="김다은">
+    <cfRule type="containsText" dxfId="43" priority="10" operator="containsText" text="김다은">
       <formula>NOT(ISERROR(SEARCH("김다은",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="48" priority="20" operator="containsText" text="취준">
+    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="취준">
       <formula>NOT(ISERROR(SEARCH("취준",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="21" operator="containsText" text="기타">
+    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="기타">
       <formula>NOT(ISERROR(SEARCH("기타",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="22" operator="containsText" text="프로젝트">
+    <cfRule type="containsText" dxfId="40" priority="24" operator="containsText" text="프로젝트">
       <formula>NOT(ISERROR(SEARCH("프로젝트",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="23" operator="containsText" text="공부">
+    <cfRule type="containsText" dxfId="39" priority="25" operator="containsText" text="공부">
       <formula>NOT(ISERROR(SEARCH("공부",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="인공지능">
+    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="선형대수">
+      <formula>NOT(ISERROR(SEARCH("선형대수",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="DX">
+      <formula>NOT(ISERROR(SEARCH("DX",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="5" operator="containsText" text="OS">
+      <formula>NOT(ISERROR(SEARCH("OS",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="PL">
+      <formula>NOT(ISERROR(SEARCH("PL",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="7" operator="containsText" text="C++">
+      <formula>NOT(ISERROR(SEARCH("C++",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="11" operator="containsText" text="인공지능">
       <formula>NOT(ISERROR(SEARCH("인공지능",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="NextJS">
+    <cfRule type="containsText" dxfId="32" priority="12" operator="containsText" text="NextJS">
       <formula>NOT(ISERROR(SEARCH("NextJS",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="지원 준비">
+    <cfRule type="containsText" dxfId="31" priority="13" operator="containsText" text="지원 준비">
       <formula>NOT(ISERROR(SEARCH("지원 준비",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="알고리즘">
+    <cfRule type="containsText" dxfId="30" priority="14" operator="containsText" text="알고리즘">
       <formula>NOT(ISERROR(SEARCH("알고리즘",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="네트워크">
+    <cfRule type="containsText" dxfId="29" priority="15" operator="containsText" text="네트워크">
       <formula>NOT(ISERROR(SEARCH("네트워크",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="자료구조">
+    <cfRule type="containsText" dxfId="28" priority="16" operator="containsText" text="자료구조">
       <formula>NOT(ISERROR(SEARCH("자료구조",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="15" operator="containsText" text="타입스크립트">
+    <cfRule type="containsText" dxfId="27" priority="17" operator="containsText" text="타입스크립트">
       <formula>NOT(ISERROR(SEARCH("타입스크립트",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="18" operator="containsText" text="기타">
+    <cfRule type="containsText" dxfId="26" priority="20" operator="containsText" text="기타">
       <formula>NOT(ISERROR(SEARCH("기타",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="C++">
-      <formula>NOT(ISERROR(SEARCH("C++",F1)))</formula>
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Computer Vision">
+      <formula>NOT(ISERROR(SEARCH("Computer Vision",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="PL">
-      <formula>NOT(ISERROR(SEARCH("PL",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="OS">
-      <formula>NOT(ISERROR(SEARCH("OS",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="DX">
-      <formula>NOT(ISERROR(SEARCH("DX",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="선형대수">
-      <formula>NOT(ISERROR(SEARCH("선형대수",F1)))</formula>
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="Game Programming">
+      <formula>NOT(ISERROR(SEARCH("Game Programming",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
@@ -5014,14 +6155,14 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="19" customWidth="1"/>
-    <col min="3" max="3" width="12.875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="16.625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12.875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -5051,7 +6192,7 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
@@ -5071,8 +6212,11 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>186</v>
       </c>
       <c r="D3" t="s">
         <v>183</v>
@@ -5088,8 +6232,11 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>187</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -5102,17 +6249,17 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="8" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="9" t="s">
         <v>138</v>
       </c>
     </row>
@@ -5122,7 +6269,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="10" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update 2024 04 17
</commit_message>
<xml_diff>
--- a/기록/Data.xlsx
+++ b/기록/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\CS_study\기록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0F3013-93D0-4900-B92F-AA4BC26B9FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DCA8015-5A54-42AC-BAC9-742B2F9E37F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="320">
   <si>
     <t>이름</t>
   </si>
@@ -1029,6 +1029,79 @@
   </si>
   <si>
     <t>프로젝트</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerActivityMonitor 캐시 최적화</t>
+  </si>
+  <si>
+    <t>Movement State 개편(더 자세하게), ActionCommand 추가 및 연결된 State, Command, Event 재작성, Command Cancel 구현중(50 %)</t>
+  </si>
+  <si>
+    <t>캡스톤 디자인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>박지훈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>리액트 딥다이브 ~1.5까지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>공부</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MDP, Bellman Euqation, Dynamic Programming 까지 정리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>캡스톤 디자인 발표 보강 및 차후 계획 보강</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한 일</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>번들러 조사</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>백준 경사로 문제 풀이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player State 처리 중 생기는 버그들 해결</t>
+  </si>
+  <si>
+    <t>오성혁</t>
+  </si>
+  <si>
+    <t>오성혁</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Player Controller 리펙토링 완료</t>
+  </si>
+  <si>
+    <t>라우팅 기능 구현 및 navigation 컴포넌트 작업</t>
+  </si>
+  <si>
+    <t>코어 JS 2장 독서 및 정리</t>
+  </si>
+  <si>
+    <t>중간고사 공부</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자소서 계기 및 사례 작성하기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2282,10 +2355,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J193"/>
+  <dimension ref="A1:J206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D215" sqref="D215"/>
+    <sheetView tabSelected="1" topLeftCell="B174" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D206" sqref="D206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6154,19 +6227,279 @@
         <v>45383</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>158</v>
+        <v>303</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>11</v>
+        <v>304</v>
       </c>
       <c r="D193" s="10" t="s">
         <v>298</v>
       </c>
       <c r="E193" s="26" t="s">
-        <v>299</v>
+        <v>254</v>
       </c>
       <c r="F193" s="27" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D194" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E194" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="F194" s="27" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A195" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D195" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="E195" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="F195" s="27" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D196" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="E196" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="F196" s="27" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D197" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="E197" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="F197" s="27" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A198" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D198" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="E198" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F198" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D199" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E199" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F199" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" s="2">
+        <v>45383</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D200" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E200" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F200" s="27" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D201" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="E201" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F201" s="27" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A202" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D202" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="E202" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F202" s="27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D203" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="E203" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F203" s="27" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A204" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D204" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="E204" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F204" s="27" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A205" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D205" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="E205" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F205" s="27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D206" s="10" t="s">
+        <v>319</v>
+      </c>
+      <c r="E206" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F206" s="27" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -6730,8 +7063,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6894,6 +7227,9 @@
       </c>
       <c r="G5" t="s">
         <v>236</v>
+      </c>
+      <c r="H5" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">

</xml_diff>